<commit_message>
Relatively stable arduino code. Can send and receive from phone and backpack
</commit_message>
<xml_diff>
--- a/Documentations/Bluetooth_Message_Definitions.xlsx
+++ b/Documentations/Bluetooth_Message_Definitions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="5820" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
   <si>
     <t>SENDER</t>
   </si>
@@ -83,6 +83,18 @@
   </si>
   <si>
     <t>(any)</t>
+  </si>
+  <si>
+    <t>glove says don't show turn signal</t>
+  </si>
+  <si>
+    <t>phone says don't show stop sign</t>
+  </si>
+  <si>
+    <t>nav says don't blink leds</t>
+  </si>
+  <si>
+    <t>disconnect</t>
   </si>
 </sst>
 </file>
@@ -527,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,88 +648,170 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="7"/>
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4">
+        <v>4</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="7"/>
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4">
+        <v>4</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="4">
+        <v>5</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="4">
+        <v>5</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C13" s="12">
         <v>1</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D13" s="13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B14" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C14" s="12">
         <v>2</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D14" s="13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-    </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="5">
-        <v>1</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="B15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="12">
+        <v>4</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="12">
+        <v>4</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="5">
+        <v>3</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="5">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="5">
+        <v>5</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B20" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C20" s="10">
         <v>9</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>